<commit_message>
Changes till May 15, 2023
</commit_message>
<xml_diff>
--- a/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/Pushnotificationdata.xlsx
+++ b/com.sevenrmartsupermarket/src/main/resources/ExcelFiles/Pushnotificationdata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krishna\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{523D8C8E-2D2C-485F-A82A-A4EF3E605896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9C29F8-961A-4C60-8455-94E08228395A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>sevenmarket</t>
   </si>
   <si>
     <t>grocery app</t>
+  </si>
+  <si>
+    <t>sevenmarket.com</t>
   </si>
 </sst>
 </file>
@@ -357,12 +354,12 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -379,7 +376,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>